<commit_message>
var now incremented when int float array or char is found
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -435,10 +435,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>

</xml_diff>